<commit_message>
Updates on the sql schema and definition of the relations between tables
</commit_message>
<xml_diff>
--- a/data/nurcara.xlsx
+++ b/data/nurcara.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3223" uniqueCount="1635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="1635">
   <si>
     <t xml:space="preserve">D'Arienzo, L.</t>
   </si>
@@ -6466,14 +6466,20 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A275"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="5" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="323.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="255.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="40.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18817,15 +18823,13 @@
   </sheetPr>
   <dimension ref="A1:A275"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A255" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A275"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A263" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A269" activeCellId="0" sqref="A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18835,417 +18839,77 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19260,652 +18924,322 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
-        <v>89</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="2" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
-        <v>1</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
-        <v>1</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
-        <v>1</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
-        <v>89</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
-        <v>89</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
-        <v>89</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="n">
-        <v>129</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
-        <v>129</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="n">
-        <v>133</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
-        <v>129</v>
+        <v>83</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="n">
-        <v>129</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="n">
-        <v>129</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2" t="n">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
-        <v>138</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
-        <v>138</v>
+        <v>85</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
-        <v>138</v>
+        <v>15</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="n">
         <v>167</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2" t="n">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="n">
         <v>169</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="n">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="n">
         <v>177</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="n">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="n">
         <v>178</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2" t="n">
-        <v>179</v>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="2" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="2" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="2" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="n">
-        <v>138</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="n">
+        <v>183</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="n">
-        <v>21</v>
+        <v>85</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2" t="n">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2" t="n">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="n">
-        <v>203</v>
+        <v>15</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="2" t="n">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="2" t="n">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="2" t="n">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="2" t="n">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="n">
-        <v>216</v>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19913,229 +19247,79 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="n">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="2" t="n">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="1" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="1" t="n">
-        <v>203</v>
-      </c>
-    </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="1" t="n">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="2" t="n">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="1" t="n">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="2" t="n">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="2" t="n">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="2" t="n">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="2" t="n">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="2" t="n">
-        <v>235</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="2" t="n">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="1" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="1" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="268" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="1" t="n">
-        <v>216</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="n">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="n">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="1" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="1" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="2" t="n">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="1" t="n">
-        <v>21</v>
+      <c r="A275" s="1" t="s">
+        <v>1633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>